<commit_message>
Added Dati anagrafici, Updated rubrica,
</commit_message>
<xml_diff>
--- a/docs/tp/BurgerMenu.xlsx
+++ b/docs/tp/BurgerMenu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953568D3-74B2-4FBE-A5F4-27AFFDEFA686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3832FDCF-4BEE-40BB-89F1-A93B5567C256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="810" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
@@ -590,18 +590,6 @@
     <t>Verifica aggancio Analisi dei bisogni</t>
   </si>
   <si>
-    <t>Verifica aggancio Ultra Casa e Patrimonio</t>
-  </si>
-  <si>
-    <t>MatrixWeb: Navigation BurgerMenuNumbers_Ultra Casa e Patrimonio</t>
-  </si>
-  <si>
-    <t>MatrixWeb: Navigation BurgerMenuNumbers_Verifica aggancio Ultra Salute</t>
-  </si>
-  <si>
-    <t>Verifica aggancio Ultra Salute</t>
-  </si>
-  <si>
     <t>Si accede a Backoffice, click burgerMenu e verifica atterraggio della pagina</t>
   </si>
   <si>
@@ -627,6 +615,18 @@
   </si>
   <si>
     <t>MatrixWeb: Navigation BurgerMenuSales_Verifica aggancio Allianz Global Assistance</t>
+  </si>
+  <si>
+    <t>Verifica aggancio New Business Ultra Salute</t>
+  </si>
+  <si>
+    <t>MatrixWeb: Navigation BurgerMenuNumbers_Verifica aggancio New Business Ultra Salute</t>
+  </si>
+  <si>
+    <t>MatrixWeb: Navigation BurgerMenuNumbers_New Business Ultra Casa e Patrimonio</t>
+  </si>
+  <si>
+    <t>Verifica aggancio New Business Ultra Casa e Patrimonio</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,10 +1763,10 @@
     </row>
     <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>29</v>
@@ -1795,10 +1795,10 @@
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>29</v>
@@ -2723,10 +2723,10 @@
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>51</v>
@@ -3075,10 +3075,10 @@
     </row>
     <row r="64" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>51</v>
@@ -3241,7 +3241,7 @@
         <v>83</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>15</v>
@@ -3273,7 +3273,7 @@
         <v>84</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>15</v>
@@ -3305,7 +3305,7 @@
         <v>85</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>15</v>
@@ -3337,7 +3337,7 @@
         <v>86</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>15</v>
@@ -3369,7 +3369,7 @@
         <v>87</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>15</v>
@@ -3401,7 +3401,7 @@
         <v>88</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>15</v>
@@ -3433,7 +3433,7 @@
         <v>89</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>15</v>
@@ -3465,7 +3465,7 @@
         <v>90</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>15</v>
@@ -3497,7 +3497,7 @@
         <v>91</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>15</v>
@@ -3529,7 +3529,7 @@
         <v>92</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>15</v>
@@ -3561,7 +3561,7 @@
         <v>93</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>15</v>
@@ -3587,13 +3587,13 @@
     </row>
     <row r="80" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>15</v>
@@ -3625,7 +3625,7 @@
         <v>94</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>15</v>
@@ -3657,7 +3657,7 @@
         <v>95</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>15</v>
@@ -3689,7 +3689,7 @@
         <v>96</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>15</v>
@@ -3721,7 +3721,7 @@
         <v>97</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>15</v>
@@ -3753,7 +3753,7 @@
         <v>98</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>15</v>
@@ -3779,13 +3779,13 @@
     </row>
     <row r="86" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Updated New Version Cancellazione Clienti nativo
</commit_message>
<xml_diff>
--- a/docs/tp/BurgerMenu.xlsx
+++ b/docs/tp/BurgerMenu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACE99DB-322A-4769-B3D4-01B91BBD1B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956574D5-4E2E-4521-8012-1ECF61195BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="810" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView minimized="1" xWindow="7470" yWindow="4215" windowWidth="14400" windowHeight="11385" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="204">
   <si>
     <t>Design</t>
   </si>
@@ -639,6 +639,12 @@
   </si>
   <si>
     <t>MatrixWeb: Navigation BurgerMenuNumbers_Verifica aggancio X - Advisor</t>
+  </si>
+  <si>
+    <t>MatrixWeb: Navigation BurgerMenuClients_Verifica aggancio Hospital scanner</t>
+  </si>
+  <si>
+    <t>Verifica aggancio Hospital scanner</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="A2:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,13 +1429,13 @@
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>203</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>15</v>
@@ -1441,7 +1447,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>12</v>
@@ -1450,18 +1456,18 @@
         <v>2</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>15</v>
@@ -1487,10 +1493,10 @@
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>29</v>
@@ -1519,10 +1525,10 @@
     </row>
     <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>29</v>
@@ -1551,10 +1557,10 @@
     </row>
     <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>201</v>
+        <v>111</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>200</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>29</v>
@@ -1583,10 +1589,10 @@
     </row>
     <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>112</v>
+        <v>201</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>29</v>
@@ -1615,10 +1621,10 @@
     </row>
     <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>29</v>
@@ -1647,10 +1653,10 @@
     </row>
     <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>29</v>
@@ -1679,10 +1685,10 @@
     </row>
     <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>29</v>
@@ -1711,10 +1717,10 @@
     </row>
     <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>29</v>
@@ -1743,10 +1749,10 @@
     </row>
     <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>29</v>
@@ -1775,10 +1781,10 @@
     </row>
     <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>29</v>
@@ -1807,10 +1813,10 @@
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>196</v>
+        <v>119</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>197</v>
+        <v>39</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>29</v>
@@ -1839,10 +1845,10 @@
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>29</v>
@@ -1871,10 +1877,10 @@
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>118</v>
+        <v>195</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>38</v>
+        <v>194</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>29</v>
@@ -1903,10 +1909,10 @@
     </row>
     <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>29</v>
@@ -1935,10 +1941,10 @@
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>29</v>
@@ -1967,10 +1973,10 @@
     </row>
     <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>29</v>
@@ -1999,10 +2005,10 @@
     </row>
     <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>29</v>
@@ -2031,10 +2037,10 @@
     </row>
     <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>29</v>
@@ -2063,10 +2069,10 @@
     </row>
     <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>29</v>
@@ -2095,10 +2101,10 @@
     </row>
     <row r="33" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>29</v>
@@ -2127,10 +2133,10 @@
     </row>
     <row r="34" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>29</v>
@@ -2159,10 +2165,10 @@
     </row>
     <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>29</v>
@@ -2191,13 +2197,13 @@
     </row>
     <row r="36" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>15</v>
@@ -2218,18 +2224,18 @@
         <v>2</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>15</v>
@@ -2255,10 +2261,10 @@
     </row>
     <row r="38" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>51</v>
@@ -2287,10 +2293,10 @@
     </row>
     <row r="39" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>51</v>
@@ -2319,10 +2325,10 @@
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>51</v>
@@ -2351,10 +2357,10 @@
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>51</v>
@@ -2383,10 +2389,10 @@
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>51</v>
@@ -2415,10 +2421,10 @@
     </row>
     <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>51</v>
@@ -2447,10 +2453,10 @@
     </row>
     <row r="44" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>51</v>
@@ -2479,10 +2485,10 @@
     </row>
     <row r="45" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>51</v>
@@ -2511,10 +2517,10 @@
     </row>
     <row r="46" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>51</v>
@@ -2543,10 +2549,10 @@
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>51</v>
@@ -2575,10 +2581,10 @@
     </row>
     <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>51</v>
@@ -2607,10 +2613,10 @@
     </row>
     <row r="49" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>51</v>
@@ -2639,10 +2645,10 @@
     </row>
     <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>199</v>
+        <v>63</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>51</v>
@@ -2671,10 +2677,10 @@
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>143</v>
+        <v>198</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>64</v>
+        <v>199</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>51</v>
@@ -2703,10 +2709,10 @@
     </row>
     <row r="52" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>51</v>
@@ -2735,10 +2741,10 @@
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>51</v>
@@ -2767,10 +2773,10 @@
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>51</v>
@@ -2799,10 +2805,10 @@
     </row>
     <row r="55" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>51</v>
@@ -2831,10 +2837,10 @@
     </row>
     <row r="56" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>51</v>
@@ -2863,10 +2869,10 @@
     </row>
     <row r="57" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>51</v>
@@ -2895,10 +2901,10 @@
     </row>
     <row r="58" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>51</v>
@@ -2927,10 +2933,10 @@
     </row>
     <row r="59" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>51</v>
@@ -2959,10 +2965,10 @@
     </row>
     <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>51</v>
@@ -2991,10 +2997,10 @@
     </row>
     <row r="61" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>51</v>
@@ -3023,10 +3029,10 @@
     </row>
     <row r="62" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>51</v>
@@ -3055,10 +3061,10 @@
     </row>
     <row r="63" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>51</v>
@@ -3087,10 +3093,10 @@
     </row>
     <row r="64" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>51</v>
@@ -3119,10 +3125,10 @@
     </row>
     <row r="65" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>51</v>
@@ -3151,10 +3157,10 @@
     </row>
     <row r="66" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>192</v>
+        <v>77</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>51</v>
@@ -3183,10 +3189,10 @@
     </row>
     <row r="67" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>78</v>
+        <v>192</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>51</v>
@@ -3215,10 +3221,10 @@
     </row>
     <row r="68" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>51</v>
@@ -3247,10 +3253,10 @@
     </row>
     <row r="69" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>51</v>
@@ -3277,15 +3283,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>15</v>
@@ -3297,7 +3303,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>12</v>
@@ -3306,18 +3312,18 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>185</v>
+        <v>82</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>15</v>
@@ -3343,10 +3349,10 @@
     </row>
     <row r="72" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>185</v>
@@ -3375,10 +3381,10 @@
     </row>
     <row r="73" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>185</v>
@@ -3407,10 +3413,10 @@
     </row>
     <row r="74" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>185</v>
@@ -3439,10 +3445,10 @@
     </row>
     <row r="75" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>185</v>
@@ -3471,10 +3477,10 @@
     </row>
     <row r="76" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>185</v>
@@ -3503,10 +3509,10 @@
     </row>
     <row r="77" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>185</v>
@@ -3535,10 +3541,10 @@
     </row>
     <row r="78" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>185</v>
@@ -3567,10 +3573,10 @@
     </row>
     <row r="79" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>185</v>
@@ -3599,10 +3605,10 @@
     </row>
     <row r="80" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>185</v>
@@ -3631,10 +3637,10 @@
     </row>
     <row r="81" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>185</v>
@@ -3663,10 +3669,10 @@
     </row>
     <row r="82" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>185</v>
@@ -3695,10 +3701,10 @@
     </row>
     <row r="83" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>185</v>
@@ -3727,10 +3733,10 @@
     </row>
     <row r="84" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>185</v>
@@ -3759,10 +3765,10 @@
     </row>
     <row r="85" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>185</v>
@@ -3791,10 +3797,10 @@
     </row>
     <row r="86" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>185</v>
@@ -3823,10 +3829,10 @@
     </row>
     <row r="87" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>185</v>
@@ -3855,10 +3861,10 @@
     </row>
     <row r="88" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>185</v>
@@ -3882,6 +3888,38 @@
         <v>2</v>
       </c>
       <c r="J88" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J89" s="4" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Ultra Impresa test on BurgerMenu and Emetti
</commit_message>
<xml_diff>
--- a/docs/tp/BurgerMenu.xlsx
+++ b/docs/tp/BurgerMenu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956574D5-4E2E-4521-8012-1ECF61195BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2753E130-2F0A-4413-A957-3BA247E947DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7470" yWindow="4215" windowWidth="14400" windowHeight="11385" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView xWindow="28680" yWindow="810" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="206">
   <si>
     <t>Design</t>
   </si>
@@ -645,6 +645,12 @@
   </si>
   <si>
     <t>Verifica aggancio Hospital scanner</t>
+  </si>
+  <si>
+    <t>MatrixWeb: Navigation BurgerMenuSales_Verifica aggancio Allianz Ultra Impresa</t>
+  </si>
+  <si>
+    <t>Verifica aggancio Allianz Ultra Impresa</t>
   </si>
 </sst>
 </file>
@@ -1055,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="A2:J12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,10 +2491,10 @@
     </row>
     <row r="45" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>51</v>
@@ -2517,10 +2523,10 @@
     </row>
     <row r="46" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>51</v>
@@ -2549,10 +2555,10 @@
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>51</v>
@@ -2581,10 +2587,10 @@
     </row>
     <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>51</v>
@@ -2613,10 +2619,10 @@
     </row>
     <row r="49" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>51</v>
@@ -2645,10 +2651,10 @@
     </row>
     <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>51</v>
@@ -2677,10 +2683,10 @@
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>199</v>
+        <v>63</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>51</v>
@@ -2709,10 +2715,10 @@
     </row>
     <row r="52" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>143</v>
+        <v>198</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>64</v>
+        <v>199</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>51</v>
@@ -2741,10 +2747,10 @@
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>51</v>
@@ -2773,10 +2779,10 @@
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>51</v>
@@ -2805,10 +2811,10 @@
     </row>
     <row r="55" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>51</v>
@@ -2837,10 +2843,10 @@
     </row>
     <row r="56" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>51</v>
@@ -2869,10 +2875,10 @@
     </row>
     <row r="57" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>51</v>
@@ -2901,10 +2907,10 @@
     </row>
     <row r="58" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>51</v>
@@ -2933,10 +2939,10 @@
     </row>
     <row r="59" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>51</v>
@@ -2965,10 +2971,10 @@
     </row>
     <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>51</v>
@@ -2997,10 +3003,10 @@
     </row>
     <row r="61" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>51</v>
@@ -3029,10 +3035,10 @@
     </row>
     <row r="62" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>51</v>
@@ -3061,10 +3067,10 @@
     </row>
     <row r="63" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>51</v>
@@ -3093,10 +3099,10 @@
     </row>
     <row r="64" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>51</v>
@@ -3125,10 +3131,10 @@
     </row>
     <row r="65" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>51</v>
@@ -3157,10 +3163,10 @@
     </row>
     <row r="66" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>51</v>
@@ -3189,10 +3195,10 @@
     </row>
     <row r="67" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>192</v>
+        <v>77</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>51</v>
@@ -3221,10 +3227,10 @@
     </row>
     <row r="68" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>78</v>
+        <v>192</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>51</v>
@@ -3253,10 +3259,10 @@
     </row>
     <row r="69" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>51</v>
@@ -3285,10 +3291,10 @@
     </row>
     <row r="70" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>51</v>
@@ -3315,15 +3321,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>15</v>
@@ -3335,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>12</v>
@@ -3344,18 +3350,18 @@
         <v>2</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>185</v>
+        <v>82</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>15</v>
@@ -3381,10 +3387,10 @@
     </row>
     <row r="73" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>185</v>
@@ -3413,10 +3419,10 @@
     </row>
     <row r="74" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>185</v>
@@ -3445,10 +3451,10 @@
     </row>
     <row r="75" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>185</v>
@@ -3477,10 +3483,10 @@
     </row>
     <row r="76" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>185</v>
@@ -3509,10 +3515,10 @@
     </row>
     <row r="77" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>185</v>
@@ -3541,10 +3547,10 @@
     </row>
     <row r="78" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>185</v>
@@ -3573,10 +3579,10 @@
     </row>
     <row r="79" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>185</v>
@@ -3605,10 +3611,10 @@
     </row>
     <row r="80" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>185</v>
@@ -3637,10 +3643,10 @@
     </row>
     <row r="81" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>185</v>
@@ -3669,10 +3675,10 @@
     </row>
     <row r="82" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>185</v>
@@ -3701,10 +3707,10 @@
     </row>
     <row r="83" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>185</v>
@@ -3733,10 +3739,10 @@
     </row>
     <row r="84" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>185</v>
@@ -3765,10 +3771,10 @@
     </row>
     <row r="85" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>185</v>
@@ -3797,10 +3803,10 @@
     </row>
     <row r="86" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>185</v>
@@ -3829,10 +3835,10 @@
     </row>
     <row r="87" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>185</v>
@@ -3861,10 +3867,10 @@
     </row>
     <row r="88" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>185</v>
@@ -3893,10 +3899,10 @@
     </row>
     <row r="89" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>185</v>
@@ -3920,6 +3926,38 @@
         <v>2</v>
       </c>
       <c r="J89" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Check Link Consensi Email sui Contratti
</commit_message>
<xml_diff>
--- a/docs/tp/BurgerMenu.xlsx
+++ b/docs/tp/BurgerMenu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2753E130-2F0A-4413-A957-3BA247E947DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42F10E1-7F3F-44B7-98C7-F3CBA0768D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="810" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="208">
   <si>
     <t>Design</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>Verifica aggancio Allianz Ultra Impresa</t>
+  </si>
+  <si>
+    <t>MatrixWeb: Navigation BurgerMenuClients_Verifica aggancio Consensi Email sui Contratti</t>
+  </si>
+  <si>
+    <t>Verifica aggancio Consensi Email sui Contratti</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,13 +1473,13 @@
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>108</v>
+        <v>206</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>15</v>
@@ -1485,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>12</v>
@@ -1494,18 +1500,18 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>15</v>
@@ -1531,10 +1537,10 @@
     </row>
     <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>29</v>
@@ -1563,10 +1569,10 @@
     </row>
     <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>29</v>
@@ -1595,10 +1601,10 @@
     </row>
     <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>201</v>
+        <v>111</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>200</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>29</v>
@@ -1627,10 +1633,10 @@
     </row>
     <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>112</v>
+        <v>201</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>29</v>
@@ -1659,10 +1665,10 @@
     </row>
     <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>29</v>
@@ -1691,10 +1697,10 @@
     </row>
     <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>29</v>
@@ -1723,10 +1729,10 @@
     </row>
     <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>29</v>
@@ -1755,10 +1761,10 @@
     </row>
     <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>29</v>
@@ -1787,10 +1793,10 @@
     </row>
     <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>29</v>
@@ -1819,10 +1825,10 @@
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>29</v>
@@ -1851,10 +1857,10 @@
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>196</v>
+        <v>119</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>197</v>
+        <v>39</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>29</v>
@@ -1883,10 +1889,10 @@
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>29</v>
@@ -1915,10 +1921,10 @@
     </row>
     <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>118</v>
+        <v>195</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>194</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>29</v>
@@ -1947,10 +1953,10 @@
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>29</v>
@@ -1979,10 +1985,10 @@
     </row>
     <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>29</v>
@@ -2011,10 +2017,10 @@
     </row>
     <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>29</v>
@@ -2043,10 +2049,10 @@
     </row>
     <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>29</v>
@@ -2075,10 +2081,10 @@
     </row>
     <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>29</v>
@@ -2107,10 +2113,10 @@
     </row>
     <row r="33" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>29</v>
@@ -2139,10 +2145,10 @@
     </row>
     <row r="34" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>29</v>
@@ -2171,10 +2177,10 @@
     </row>
     <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>29</v>
@@ -2203,10 +2209,10 @@
     </row>
     <row r="36" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>29</v>
@@ -2235,13 +2241,13 @@
     </row>
     <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>15</v>
@@ -2262,18 +2268,18 @@
         <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>15</v>
@@ -2299,10 +2305,10 @@
     </row>
     <row r="39" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>51</v>
@@ -2331,10 +2337,10 @@
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>51</v>
@@ -2363,10 +2369,10 @@
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>51</v>
@@ -2395,10 +2401,10 @@
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>51</v>
@@ -2427,10 +2433,10 @@
     </row>
     <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>51</v>
@@ -2459,10 +2465,10 @@
     </row>
     <row r="44" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>51</v>
@@ -2491,10 +2497,10 @@
     </row>
     <row r="45" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>204</v>
+        <v>135</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>205</v>
+        <v>56</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>51</v>
@@ -2523,10 +2529,10 @@
     </row>
     <row r="46" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>51</v>
@@ -2555,10 +2561,10 @@
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>51</v>
@@ -2587,10 +2593,10 @@
     </row>
     <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>51</v>
@@ -2619,10 +2625,10 @@
     </row>
     <row r="49" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>51</v>
@@ -2651,10 +2657,10 @@
     </row>
     <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>51</v>
@@ -2683,10 +2689,10 @@
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>51</v>
@@ -2715,10 +2721,10 @@
     </row>
     <row r="52" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>199</v>
+        <v>63</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>51</v>
@@ -2747,10 +2753,10 @@
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>143</v>
+        <v>198</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>64</v>
+        <v>199</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>51</v>
@@ -2779,10 +2785,10 @@
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>51</v>
@@ -2811,10 +2817,10 @@
     </row>
     <row r="55" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>51</v>
@@ -2843,10 +2849,10 @@
     </row>
     <row r="56" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>51</v>
@@ -2875,10 +2881,10 @@
     </row>
     <row r="57" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>51</v>
@@ -2907,10 +2913,10 @@
     </row>
     <row r="58" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>51</v>
@@ -2939,10 +2945,10 @@
     </row>
     <row r="59" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>51</v>
@@ -2971,10 +2977,10 @@
     </row>
     <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>51</v>
@@ -3003,10 +3009,10 @@
     </row>
     <row r="61" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>51</v>
@@ -3035,10 +3041,10 @@
     </row>
     <row r="62" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>51</v>
@@ -3067,10 +3073,10 @@
     </row>
     <row r="63" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>51</v>
@@ -3099,10 +3105,10 @@
     </row>
     <row r="64" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>51</v>
@@ -3131,10 +3137,10 @@
     </row>
     <row r="65" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>51</v>
@@ -3163,10 +3169,10 @@
     </row>
     <row r="66" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>51</v>
@@ -3195,10 +3201,10 @@
     </row>
     <row r="67" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>51</v>
@@ -3227,10 +3233,10 @@
     </row>
     <row r="68" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>192</v>
+        <v>77</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>51</v>
@@ -3259,10 +3265,10 @@
     </row>
     <row r="69" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>78</v>
+        <v>192</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>51</v>
@@ -3291,10 +3297,10 @@
     </row>
     <row r="70" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>51</v>
@@ -3323,10 +3329,10 @@
     </row>
     <row r="71" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>51</v>
@@ -3353,15 +3359,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>15</v>
@@ -3373,7 +3379,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>12</v>
@@ -3382,18 +3388,18 @@
         <v>2</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>185</v>
+        <v>82</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>15</v>
@@ -3419,10 +3425,10 @@
     </row>
     <row r="74" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>185</v>
@@ -3451,10 +3457,10 @@
     </row>
     <row r="75" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>185</v>
@@ -3483,10 +3489,10 @@
     </row>
     <row r="76" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>185</v>
@@ -3515,10 +3521,10 @@
     </row>
     <row r="77" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>185</v>
@@ -3547,10 +3553,10 @@
     </row>
     <row r="78" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>185</v>
@@ -3579,10 +3585,10 @@
     </row>
     <row r="79" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>185</v>
@@ -3611,10 +3617,10 @@
     </row>
     <row r="80" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>185</v>
@@ -3643,10 +3649,10 @@
     </row>
     <row r="81" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>185</v>
@@ -3675,10 +3681,10 @@
     </row>
     <row r="82" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>185</v>
@@ -3707,10 +3713,10 @@
     </row>
     <row r="83" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>185</v>
@@ -3739,10 +3745,10 @@
     </row>
     <row r="84" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>185</v>
@@ -3771,10 +3777,10 @@
     </row>
     <row r="85" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>185</v>
@@ -3803,10 +3809,10 @@
     </row>
     <row r="86" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>185</v>
@@ -3835,10 +3841,10 @@
     </row>
     <row r="87" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>185</v>
@@ -3867,10 +3873,10 @@
     </row>
     <row r="88" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>185</v>
@@ -3899,10 +3905,10 @@
     </row>
     <row r="89" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>185</v>
@@ -3931,10 +3937,10 @@
     </row>
     <row r="90" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>185</v>
@@ -3958,6 +3964,38 @@
         <v>2</v>
       </c>
       <c r="J90" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Link Gestione Certificati + TP updated
</commit_message>
<xml_diff>
--- a/docs/tp/BurgerMenu.xlsx
+++ b/docs/tp/BurgerMenu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42F10E1-7F3F-44B7-98C7-F3CBA0768D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067281CE-07DB-4045-8E4A-6B0934275571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="210">
   <si>
     <t>Design</t>
   </si>
@@ -657,6 +657,12 @@
   </si>
   <si>
     <t>Verifica aggancio Consensi Email sui Contratti</t>
+  </si>
+  <si>
+    <t>MatrixWeb: Navigation BurgerMenuNumbers_Verifica aggancio New Business Ultra Impresa</t>
+  </si>
+  <si>
+    <t>Verifica aggancio New Business Ultra Impresa</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,10 +1959,10 @@
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>38</v>
+        <v>209</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>29</v>
@@ -1985,10 +1991,10 @@
     </row>
     <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>29</v>
@@ -2017,10 +2023,10 @@
     </row>
     <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>29</v>
@@ -2049,10 +2055,10 @@
     </row>
     <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>29</v>
@@ -2081,10 +2087,10 @@
     </row>
     <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>29</v>
@@ -2113,10 +2119,10 @@
     </row>
     <row r="33" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>29</v>
@@ -2145,10 +2151,10 @@
     </row>
     <row r="34" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>29</v>
@@ -2177,10 +2183,10 @@
     </row>
     <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>29</v>
@@ -2209,10 +2215,10 @@
     </row>
     <row r="36" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>29</v>
@@ -2241,10 +2247,10 @@
     </row>
     <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>29</v>
@@ -2273,13 +2279,13 @@
     </row>
     <row r="38" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>15</v>
@@ -2300,18 +2306,18 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>15</v>
@@ -2337,10 +2343,10 @@
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>51</v>
@@ -2369,10 +2375,10 @@
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>51</v>
@@ -2401,10 +2407,10 @@
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>51</v>
@@ -2433,10 +2439,10 @@
     </row>
     <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>51</v>
@@ -2465,10 +2471,10 @@
     </row>
     <row r="44" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>51</v>
@@ -2497,10 +2503,10 @@
     </row>
     <row r="45" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>51</v>
@@ -2529,10 +2535,10 @@
     </row>
     <row r="46" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>204</v>
+        <v>135</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>205</v>
+        <v>56</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>51</v>
@@ -2561,10 +2567,10 @@
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>51</v>
@@ -2593,10 +2599,10 @@
     </row>
     <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>51</v>
@@ -2625,10 +2631,10 @@
     </row>
     <row r="49" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>51</v>
@@ -2657,10 +2663,10 @@
     </row>
     <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>51</v>
@@ -2689,10 +2695,10 @@
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>51</v>
@@ -2721,10 +2727,10 @@
     </row>
     <row r="52" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>51</v>
@@ -2753,10 +2759,10 @@
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>199</v>
+        <v>63</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>51</v>
@@ -2785,10 +2791,10 @@
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>143</v>
+        <v>198</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>64</v>
+        <v>199</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>51</v>
@@ -2817,10 +2823,10 @@
     </row>
     <row r="55" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>51</v>
@@ -2849,10 +2855,10 @@
     </row>
     <row r="56" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>51</v>
@@ -2881,10 +2887,10 @@
     </row>
     <row r="57" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>51</v>
@@ -2913,10 +2919,10 @@
     </row>
     <row r="58" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>51</v>
@@ -2945,10 +2951,10 @@
     </row>
     <row r="59" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>51</v>
@@ -2977,10 +2983,10 @@
     </row>
     <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>51</v>
@@ -3009,10 +3015,10 @@
     </row>
     <row r="61" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>51</v>
@@ -3041,10 +3047,10 @@
     </row>
     <row r="62" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>51</v>
@@ -3073,10 +3079,10 @@
     </row>
     <row r="63" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>51</v>
@@ -3105,10 +3111,10 @@
     </row>
     <row r="64" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>51</v>
@@ -3137,10 +3143,10 @@
     </row>
     <row r="65" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>51</v>
@@ -3169,10 +3175,10 @@
     </row>
     <row r="66" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>51</v>
@@ -3201,10 +3207,10 @@
     </row>
     <row r="67" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>51</v>
@@ -3233,10 +3239,10 @@
     </row>
     <row r="68" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>51</v>
@@ -3265,10 +3271,10 @@
     </row>
     <row r="69" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>192</v>
+        <v>77</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>51</v>
@@ -3297,10 +3303,10 @@
     </row>
     <row r="70" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>78</v>
+        <v>192</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>51</v>
@@ -3329,10 +3335,10 @@
     </row>
     <row r="71" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>51</v>
@@ -3361,10 +3367,10 @@
     </row>
     <row r="72" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>51</v>
@@ -3391,15 +3397,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>15</v>
@@ -3411,7 +3417,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>12</v>
@@ -3420,18 +3426,18 @@
         <v>2</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>185</v>
+        <v>82</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>15</v>
@@ -3457,10 +3463,10 @@
     </row>
     <row r="75" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>185</v>
@@ -3489,10 +3495,10 @@
     </row>
     <row r="76" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>185</v>
@@ -3521,10 +3527,10 @@
     </row>
     <row r="77" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>185</v>
@@ -3553,10 +3559,10 @@
     </row>
     <row r="78" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>185</v>
@@ -3585,10 +3591,10 @@
     </row>
     <row r="79" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>185</v>
@@ -3617,10 +3623,10 @@
     </row>
     <row r="80" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>185</v>
@@ -3649,10 +3655,10 @@
     </row>
     <row r="81" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>185</v>
@@ -3681,10 +3687,10 @@
     </row>
     <row r="82" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>185</v>
@@ -3713,10 +3719,10 @@
     </row>
     <row r="83" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>185</v>
@@ -3745,10 +3751,10 @@
     </row>
     <row r="84" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>185</v>
@@ -3777,10 +3783,10 @@
     </row>
     <row r="85" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>185</v>
@@ -3809,10 +3815,10 @@
     </row>
     <row r="86" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>185</v>
@@ -3841,10 +3847,10 @@
     </row>
     <row r="87" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>185</v>
@@ -3873,10 +3879,10 @@
     </row>
     <row r="88" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>185</v>
@@ -3905,10 +3911,10 @@
     </row>
     <row r="89" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>185</v>
@@ -3937,10 +3943,10 @@
     </row>
     <row r="90" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>185</v>
@@ -3969,10 +3975,10 @@
     </row>
     <row r="91" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>185</v>
@@ -3996,6 +4002,38 @@
         <v>2</v>
       </c>
       <c r="J91" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J92" s="4" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>